<commit_message>
✅ Freeze ejecutado: roster y freeze_time actualizados
</commit_message>
<xml_diff>
--- a/data/processed/daily_rosters_excels/roster_2025-10-22.xlsx
+++ b/data/processed/daily_rosters_excels/roster_2025-10-22.xlsx
@@ -870,26 +870,26 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>3133603</v>
+        <v>4433247</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Kelly Oubre Jr.</t>
+          <t>Jonathan Kuminga</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>GSW</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>SF</t>
+          <t>PF</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>1626162</t>
+          <t>1630228</t>
         </is>
       </c>
     </row>
@@ -908,26 +908,26 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>4433247</v>
+        <v>3907497</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Jonathan Kuminga</t>
+          <t>Dejounte Murray</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>GSW</t>
+          <t>NOP</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>PF</t>
+          <t>SG</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>1630228</t>
+          <t>1627749</t>
         </is>
       </c>
     </row>
@@ -946,26 +946,26 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>3907497</v>
+        <v>3448</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Dejounte Murray</t>
+          <t>Brook Lopez</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>NOP</t>
+          <t>LAC</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>SG</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>1627749</t>
+          <t>201572</t>
         </is>
       </c>
     </row>
@@ -984,26 +984,26 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>3448</v>
+        <v>5124612</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Brook Lopez</t>
+          <t>VJ Edgecombe</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>LAC</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>SG</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>201572</t>
+          <t>1642845</t>
         </is>
       </c>
     </row>
@@ -1516,26 +1516,26 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>6475</v>
+        <v>4432165</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Klay Thompson</t>
+          <t>Jalen Suggs</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>DAL</t>
+          <t>ORL</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>SG</t>
+          <t>PG</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>202691</t>
+          <t>1630591</t>
         </is>
       </c>
     </row>
@@ -5126,26 +5126,26 @@
         </is>
       </c>
       <c r="D124" t="n">
-        <v>3934673</v>
+        <v>5037871</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>Donte DiVincenzo</t>
+          <t>Dylan Harper</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>SAS</t>
         </is>
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>SG</t>
+          <t>PG</t>
         </is>
       </c>
       <c r="H124" t="inlineStr">
         <is>
-          <t>1628978</t>
+          <t>1642844</t>
         </is>
       </c>
     </row>
@@ -5164,26 +5164,26 @@
         </is>
       </c>
       <c r="D125" t="n">
-        <v>5037871</v>
+        <v>4396909</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>Dylan Harper</t>
+          <t>Aaron Nesmith</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>PG</t>
+          <t>SF</t>
         </is>
       </c>
       <c r="H125" t="inlineStr">
         <is>
-          <t>1642844</t>
+          <t>1630174</t>
         </is>
       </c>
     </row>

</xml_diff>